<commit_message>
Información de aves, casos de prueba completos
</commit_message>
<xml_diff>
--- a/Casos de prueba.xlsx
+++ b/Casos de prueba.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Dropbox\II Semestre 2017\Bases de Datos I\Proyecto 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\BirdLand\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="111">
   <si>
     <t>Casos de prueba</t>
   </si>
@@ -139,21 +139,6 @@
     <t>Se pueden realizar consultas por  aves registradas por persona</t>
   </si>
   <si>
-    <r>
-      <t>Se muestran estadísticas de  la cantidad de aves registradas por orden</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (con el listado)</t>
-    </r>
-  </si>
-  <si>
     <t>Se muestran estadísticas de  la cantidad de aves registradas por suborden</t>
   </si>
   <si>
@@ -178,27 +163,18 @@
     <t>Se muestra un mapa de google maps con los avistamientos</t>
   </si>
   <si>
-    <t>Las localizaciones mostradas en el mapa están acorden con las ingresadas al realizar el avistamiento</t>
-  </si>
-  <si>
     <t xml:space="preserve">Al modificar los filtros el mapa refresca con los nuevos puntos </t>
   </si>
   <si>
     <t>En la visualización del mapa es posible utilizar filtros</t>
   </si>
   <si>
-    <t>El sistema identifica los avistamientos de aves en peligro de extincción</t>
-  </si>
-  <si>
     <t>Se realiza un reporte de los avistamientos en los que las aves estén en peligro de extinción</t>
   </si>
   <si>
     <t>El sistema envía un correo electrónico a los usuarios en su día de cumpleaños</t>
   </si>
   <si>
-    <t>El proceso de de correos electrónicos se realiza por medio de un job a media noche todos los días</t>
-  </si>
-  <si>
     <t>Se tiene una bitácora con los cambios de clave realizados por los usuarios</t>
   </si>
   <si>
@@ -208,9 +184,6 @@
     <t>La paginación es parametrizable</t>
   </si>
   <si>
-    <t>El sistema incluye la información de las familias Furnariidae y Incertae sedis</t>
-  </si>
-  <si>
     <t>El sistema incluye la información de las localizaciones del país</t>
   </si>
   <si>
@@ -260,6 +233,138 @@
   </si>
   <si>
     <t>Se pueden crear avistamientos sin fotos</t>
+  </si>
+  <si>
+    <t>Se muestra un mapa que permite marcar la localización del avistamiento</t>
+  </si>
+  <si>
+    <t>Se muestra entre las características del ave, si está o no en peligro de extinción</t>
+  </si>
+  <si>
+    <t>No es posible realizar un avistamiento sin haber elegido el avistada</t>
+  </si>
+  <si>
+    <t>Se muestra entre las características del ave</t>
+  </si>
+  <si>
+    <t>Se muestra todas la aves que pertenecen a ese orden</t>
+  </si>
+  <si>
+    <t>Se muestra todas la aves que pertenecen a ese suborden</t>
+  </si>
+  <si>
+    <t>Se muestra todas la aves que pertenecen a ese especie</t>
+  </si>
+  <si>
+    <t>Se muestra todas la aves que pertenecen a esa familia</t>
+  </si>
+  <si>
+    <t>Se muestra todas la aves que pertenecen a ese género</t>
+  </si>
+  <si>
+    <t>Se muestran las aves que tienen ese color</t>
+  </si>
+  <si>
+    <t>Se muestran estadísticas de  la cantidad de aves registradas por orden</t>
+  </si>
+  <si>
+    <t>Se muestra todas la aves que viven en esa ubicación</t>
+  </si>
+  <si>
+    <t>Se muestra todas la aves registradas por cada persona</t>
+  </si>
+  <si>
+    <t>Se muestra todas la aves que tienen cierto tamaño</t>
+  </si>
+  <si>
+    <t>Hay un acceso a una ficha técnica que muestra los datos</t>
+  </si>
+  <si>
+    <t>Se da el número exacto de aves registradas por orden</t>
+  </si>
+  <si>
+    <t>Se da el número exacto de aves registradas por suborden</t>
+  </si>
+  <si>
+    <t>Se da el número exacto de aves registradas por familia</t>
+  </si>
+  <si>
+    <t>Se da el número exacto de aves registradas por género</t>
+  </si>
+  <si>
+    <t>Se da el número exacto de aves registradas por especie</t>
+  </si>
+  <si>
+    <t>Se da el número exacto de aves registradas por zona de vida</t>
+  </si>
+  <si>
+    <t>Top 5 de las personas con mayor cantidad de avistamientos</t>
+  </si>
+  <si>
+    <t>Top 5 de los avistamientos con mayor puntuación</t>
+  </si>
+  <si>
+    <t>Las localizaciones mostradas en el mapa están acorde con las ingresadas al realizar el avistamiento</t>
+  </si>
+  <si>
+    <t>En el mapa se utilizan marcadores en la ubicaión donde se realizó cada avistamiento</t>
+  </si>
+  <si>
+    <t>Los marcadores son certeros</t>
+  </si>
+  <si>
+    <t>Se utilizan filtros para mostrar solo la información que el usuario pide</t>
+  </si>
+  <si>
+    <t>Filtros funcionales</t>
+  </si>
+  <si>
+    <t>El sistema identifica los avistamientos de aves en peligro de extinción</t>
+  </si>
+  <si>
+    <t>Las aves se catalogan si están en peligro de extinción o no.</t>
+  </si>
+  <si>
+    <t>Se muestra un reporte, para los administradores, de todos los avistamentos  de aves en peligro de extinción</t>
+  </si>
+  <si>
+    <t>Correo electrónico a los cumpleañeros</t>
+  </si>
+  <si>
+    <t>El proceso de de correos electrónicos se realiza por medio de un job, a media noche todos los días</t>
+  </si>
+  <si>
+    <t>El envío de correos se realiza en un tiempo establecido</t>
+  </si>
+  <si>
+    <t>Cada vez que un usuario cambia su clave, estos cambios se registran en una bitácora</t>
+  </si>
+  <si>
+    <t>El mensaje del correo de cumpleaños puede ser cambiado por el administrador</t>
+  </si>
+  <si>
+    <t>La cantidad de registros que se muestran por página puede ser cambiado por el administrador</t>
+  </si>
+  <si>
+    <t>El sistema viene cargado, como mínimo, con las aves pertenecientes a las familias Furnariidae e Incertae sedis</t>
+  </si>
+  <si>
+    <t>El sistema incluye la información de las familias Furnariidae e Incertae sedis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se encuetra disponible la información de todos los distritos, cantones y provincias del país </t>
+  </si>
+  <si>
+    <t>Se registra en base de datos que usuario realizó cada cambio en el sistema</t>
+  </si>
+  <si>
+    <t>Al diseñar e implementar las tablas se siguieron las reglas de normalización</t>
+  </si>
+  <si>
+    <t>Se modularizan las funciones y procedimientos dentro de paquetes</t>
+  </si>
+  <si>
+    <t>Los procedimientos y funciones son almacenados.</t>
   </si>
 </sst>
 </file>
@@ -267,6 +372,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,21 +405,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -337,43 +442,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1146,7 +1255,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
@@ -1154,26 +1263,26 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="8">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="3">
         <v>50</v>
       </c>
     </row>
@@ -1186,681 +1295,760 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="108.85546875" customWidth="1"/>
-    <col min="4" max="4" width="91" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="6" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="108.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="91" style="6" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G3" s="2"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="4">
+      <c r="B5" s="8">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="8">
+        <v>2</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="8">
+        <v>3</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="8">
+        <v>4</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="8">
+        <v>5</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="8">
+        <v>6</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="8">
+        <v>7</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="E11" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="8">
+        <v>8</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="8">
+        <v>9</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="8">
+        <v>10</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="8">
+        <v>11</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="8">
+        <v>12</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="8">
+        <v>13</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="11">
+        <v>14</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="11">
+        <v>15</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="11">
+        <v>16</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="11">
+        <v>17</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="11">
+        <v>18</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="11">
+        <v>19</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="4">
-        <v>2</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="4">
-        <v>3</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="4">
-        <v>4</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="4">
-        <v>5</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="4">
-        <v>6</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="4">
-        <v>7</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="4">
-        <v>8</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="4">
-        <v>9</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="4">
-        <v>10</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="4">
-        <v>11</v>
-      </c>
-      <c r="C15" s="5" t="s">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="11">
         <v>20</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="4">
-        <v>12</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="C24" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="11">
         <v>21</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="4">
-        <v>13</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="C25" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="11">
         <v>22</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="12">
-        <v>14</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="C26" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="11">
         <v>23</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="12">
-        <v>15</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="C27" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="11">
         <v>24</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="12">
-        <v>16</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="C28" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="11">
+        <v>25</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="11">
         <v>26</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="12">
-        <v>17</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="C30" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="11">
         <v>27</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="12">
-        <v>18</v>
-      </c>
-      <c r="C22" s="5" t="s">
+      <c r="C31" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="11">
         <v>28</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="12">
-        <v>19</v>
-      </c>
-      <c r="C23" s="5" t="s">
+      <c r="C32" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="11">
         <v>29</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="12">
-        <v>20</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="12">
-        <v>21</v>
-      </c>
-      <c r="C25" s="5" t="s">
+      <c r="C33" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="11">
         <v>30</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="12">
-        <v>22</v>
-      </c>
-      <c r="C26" s="5" t="s">
+      <c r="C34" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="11">
         <v>31</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="12">
-        <v>23</v>
-      </c>
-      <c r="C27" s="5" t="s">
+      <c r="C35" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="11">
         <v>32</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="12">
-        <v>24</v>
-      </c>
-      <c r="C28" s="5" t="s">
+      <c r="C36" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="12">
+        <v>33</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="12">
         <v>34</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="12">
-        <v>25</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="12">
-        <v>26</v>
-      </c>
-      <c r="C30" s="5" t="s">
+      <c r="C38" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="12">
         <v>35</v>
       </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="12">
-        <v>27</v>
-      </c>
-      <c r="C31" s="5" t="s">
+      <c r="C39" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="12">
         <v>36</v>
       </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="12">
-        <v>28</v>
-      </c>
-      <c r="C32" s="5" t="s">
+      <c r="C40" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="12">
         <v>37</v>
       </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="12">
-        <v>29</v>
-      </c>
-      <c r="C33" s="5" t="s">
+      <c r="C41" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="12">
         <v>38</v>
       </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="12">
-        <v>30</v>
-      </c>
-      <c r="C34" s="5" t="s">
+      <c r="C42" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="12">
         <v>39</v>
       </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="12">
-        <v>31</v>
-      </c>
-      <c r="C35" s="5" t="s">
+      <c r="C43" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="12">
         <v>40</v>
       </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="12">
-        <v>32</v>
-      </c>
-      <c r="C36" s="5" t="s">
+      <c r="C44" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="12">
         <v>41</v>
       </c>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="13">
-        <v>33</v>
-      </c>
-      <c r="C37" s="5" t="s">
+      <c r="C45" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="12">
         <v>42</v>
       </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="13">
-        <v>34</v>
-      </c>
-      <c r="C38" s="5" t="s">
+      <c r="C46" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="12">
         <v>43</v>
       </c>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="13">
-        <v>35</v>
-      </c>
-      <c r="C39" s="5" t="s">
+      <c r="C47" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="12">
         <v>44</v>
       </c>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="13">
-        <v>36</v>
-      </c>
-      <c r="C40" s="5" t="s">
+      <c r="C48" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B49" s="12">
+        <v>45</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="12">
         <v>46</v>
       </c>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="13">
-        <v>37</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="13">
-        <v>38</v>
-      </c>
-      <c r="C42" s="10" t="s">
+      <c r="C50" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="12">
         <v>47</v>
       </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="13">
-        <v>39</v>
-      </c>
-      <c r="C43" s="10" t="s">
+      <c r="C51" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="12">
         <v>48</v>
       </c>
-      <c r="D43" s="10"/>
-      <c r="E43" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="13">
-        <v>40</v>
-      </c>
-      <c r="C44" s="10" t="s">
+      <c r="C52" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="12">
         <v>49</v>
       </c>
-      <c r="D44" s="10"/>
-      <c r="E44" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="13">
-        <v>41</v>
-      </c>
-      <c r="C45" s="10" t="s">
+      <c r="C53" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="12">
         <v>50</v>
       </c>
-      <c r="D45" s="10"/>
-      <c r="E45" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="13">
-        <v>42</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D46" s="10"/>
-      <c r="E46" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="13">
-        <v>43</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="13">
-        <v>44</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D48" s="10"/>
-      <c r="E48" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="13">
-        <v>45</v>
-      </c>
-      <c r="C49" s="10" t="s">
+      <c r="C54" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D49" s="10"/>
-      <c r="E49" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="13">
-        <v>46</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D50" s="10"/>
-      <c r="E50" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="13">
-        <v>47</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D51" s="10"/>
-      <c r="E51" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="13">
-        <v>48</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D52" s="10"/>
-      <c r="E52" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="13">
-        <v>49</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D53" s="10"/>
-      <c r="E53" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="13">
-        <v>50</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D54" s="10"/>
+      <c r="D54" s="13" t="s">
+        <v>109</v>
+      </c>
       <c r="E54" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
+      <c r="B60" s="15"/>
+      <c r="C60" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>